<commit_message>
Rel 1.1 v7 Kaleido + updated raw SCH
</commit_message>
<xml_diff>
--- a/versions/v7-kaleido-34/fabrication/v7-kaleido-all-pos.xlsx
+++ b/versions/v7-kaleido-34/fabrication/v7-kaleido-all-pos.xlsx
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
+  <si>
+    <t>Designator</t>
+  </si>
   <si>
     <t>top</t>
   </si>
@@ -109,10 +112,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A59" sqref="A59:XFD59"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -121,14 +124,12 @@
     <col min="2" max="2" style="0" width="11.570733173076924" bestFit="1" customWidth="1"/>
     <col min="3" max="3" style="0" width="13.14206730769231" bestFit="1" customWidth="1"/>
     <col min="4" max="4" style="0" width="11.999278846153848" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" style="0" width="9.142307692307693"/>
+    <col min="5" max="256" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Designator</t>
-        </is>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
@@ -167,7 +168,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5">
@@ -186,7 +187,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.5">
@@ -205,7 +206,7 @@
         <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.5">
@@ -224,7 +225,7 @@
         <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.5">
@@ -243,7 +244,7 @@
         <v>-90</v>
       </c>
       <c r="E6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5">
@@ -262,7 +263,7 @@
         <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.5">
@@ -281,7 +282,7 @@
         <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.5">
@@ -300,7 +301,7 @@
         <v>180</v>
       </c>
       <c r="E9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.5">
@@ -319,7 +320,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.5">
@@ -338,7 +339,7 @@
         <v>-90</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.5">
@@ -357,7 +358,7 @@
         <v>180</v>
       </c>
       <c r="E12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.5">
@@ -376,7 +377,7 @@
         <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.5">
@@ -395,7 +396,7 @@
         <v>180</v>
       </c>
       <c r="E14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.5">
@@ -414,7 +415,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.5">
@@ -433,7 +434,7 @@
         <v>-90</v>
       </c>
       <c r="E16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.5">
@@ -452,7 +453,7 @@
         <v>90</v>
       </c>
       <c r="E17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="13.5">
@@ -471,7 +472,7 @@
         <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="13.5">
@@ -490,7 +491,7 @@
         <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.5">
@@ -509,7 +510,7 @@
         <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="13.5">
@@ -528,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="13.5">
@@ -547,7 +548,7 @@
         <v>-90</v>
       </c>
       <c r="E22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="13.5">
@@ -566,7 +567,7 @@
         <v>-90</v>
       </c>
       <c r="E23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="13.5">
@@ -585,7 +586,7 @@
         <v>90</v>
       </c>
       <c r="E24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="13.5">
@@ -604,7 +605,7 @@
         <v>90</v>
       </c>
       <c r="E25" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.5">
@@ -623,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="13.5">
@@ -642,7 +643,7 @@
         <v>90</v>
       </c>
       <c r="E27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="13.5">
@@ -661,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="13.5">
@@ -680,7 +681,7 @@
         <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="13.5">
@@ -699,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="13.5">
@@ -718,7 +719,7 @@
         <v>180</v>
       </c>
       <c r="E31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="13.5">
@@ -737,7 +738,7 @@
         <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="13.5">
@@ -756,7 +757,7 @@
         <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13.5">
@@ -775,7 +776,7 @@
         <v>180</v>
       </c>
       <c r="E34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="13.5">
@@ -794,7 +795,7 @@
         <v>90</v>
       </c>
       <c r="E35" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="13.5">
@@ -813,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="13.5">
@@ -832,7 +833,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="13.5">
@@ -851,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="13.5">
@@ -870,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="13.5">
@@ -889,7 +890,7 @@
         <v>-90</v>
       </c>
       <c r="E40" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="13.5">
@@ -908,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="13.5">
@@ -927,7 +928,7 @@
         <v>-90</v>
       </c>
       <c r="E42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="13.5">
@@ -946,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="13.5">
@@ -956,16 +957,16 @@
         </is>
       </c>
       <c r="B44" s="3">
-        <v>159.15000000000001</v>
+        <v>170.63</v>
       </c>
       <c r="C44" s="3">
-        <v>-93.209999999999994</v>
+        <v>-98.340000000000003</v>
       </c>
       <c r="D44" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="13.5">
@@ -975,1365 +976,1479 @@
         </is>
       </c>
       <c r="B45" s="3">
-        <v>171.85249999999999</v>
+        <v>171</v>
       </c>
       <c r="C45" s="3">
-        <v>-91.359999999999999</v>
+        <v>-88.890000000000001</v>
       </c>
       <c r="D45" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.5">
       <c r="A46" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>C45</t>
         </is>
       </c>
       <c r="B46" s="3">
-        <v>99.358500000000006</v>
+        <v>157.19999999999999</v>
       </c>
       <c r="C46" s="3">
-        <v>-120.681693</v>
+        <v>-98.340000000000003</v>
       </c>
       <c r="D46" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="13.5">
       <c r="A47" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>C46</t>
         </is>
       </c>
       <c r="B47" s="3">
-        <v>88.436499999999995</v>
+        <v>157.75999999999999</v>
       </c>
       <c r="C47" s="3">
-        <v>-126.52369299999999</v>
+        <v>-88.890000000000001</v>
       </c>
       <c r="D47" s="3">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="13.5">
       <c r="A48" t="inlineStr">
         <is>
-          <t>D3</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="B48" s="3">
-        <v>85.896500000000003</v>
+        <v>99.358500000000006</v>
       </c>
       <c r="C48" s="3">
-        <v>-126.52369299999999</v>
+        <v>-120.681693</v>
       </c>
       <c r="D48" s="3">
         <v>-90</v>
       </c>
       <c r="E48" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="13.5">
       <c r="A49" t="inlineStr">
         <is>
-          <t>D4</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="B49" s="3">
-        <v>99.485500000000002</v>
+        <v>88.436499999999995</v>
       </c>
       <c r="C49" s="3">
-        <v>-138.33469299999999</v>
+        <v>-126.52369299999999</v>
       </c>
       <c r="D49" s="3">
         <v>90</v>
       </c>
       <c r="E49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="13.5">
       <c r="A50" t="inlineStr">
         <is>
-          <t>D5</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="B50" s="3">
-        <v>88.436499999999995</v>
+        <v>85.896500000000003</v>
       </c>
       <c r="C50" s="3">
-        <v>-135.66769300000001</v>
+        <v>-126.52369299999999</v>
       </c>
       <c r="D50" s="3">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E50" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13.5">
       <c r="A51" t="inlineStr">
         <is>
-          <t>D6</t>
+          <t>D4</t>
         </is>
       </c>
       <c r="B51" s="3">
-        <v>85.896500000000003</v>
+        <v>99.485500000000002</v>
       </c>
       <c r="C51" s="3">
-        <v>-135.66769300000001</v>
+        <v>-138.33469299999999</v>
       </c>
       <c r="D51" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E51" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13.5">
       <c r="A52" t="inlineStr">
         <is>
-          <t>D7</t>
+          <t>D5</t>
         </is>
       </c>
       <c r="B52" s="3">
-        <v>63.596499999999999</v>
+        <v>88.436499999999995</v>
       </c>
       <c r="C52" s="3">
-        <v>-125.943693</v>
+        <v>-135.66769300000001</v>
       </c>
       <c r="D52" s="3">
         <v>90</v>
       </c>
       <c r="E52" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="13.5">
       <c r="A53" t="inlineStr">
         <is>
-          <t>D8</t>
+          <t>D6</t>
         </is>
       </c>
       <c r="B53" s="3">
-        <v>72.141499999999994</v>
+        <v>85.896500000000003</v>
       </c>
       <c r="C53" s="3">
-        <v>-143.94319300000001</v>
+        <v>-135.66769300000001</v>
       </c>
       <c r="D53" s="3">
         <v>-90</v>
       </c>
       <c r="E53" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="13.5">
       <c r="A54" t="inlineStr">
         <is>
-          <t>D9</t>
+          <t>D7</t>
         </is>
       </c>
       <c r="B54" s="3">
-        <v>74.554500000000004</v>
+        <v>63.596499999999999</v>
       </c>
       <c r="C54" s="3">
-        <v>-143.94319300000001</v>
+        <v>-125.943693</v>
       </c>
       <c r="D54" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E54" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="13.5">
       <c r="A55" t="inlineStr">
         <is>
-          <t>D10</t>
+          <t>D8</t>
         </is>
       </c>
       <c r="B55" s="3">
-        <v>70.796499999999995</v>
+        <v>72.141499999999994</v>
       </c>
       <c r="C55" s="3">
-        <v>-124.543693</v>
+        <v>-143.94319300000001</v>
       </c>
       <c r="D55" s="3">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E55" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="13.5">
       <c r="A56" t="inlineStr">
         <is>
-          <t>D11</t>
+          <t>D9</t>
         </is>
       </c>
       <c r="B56" s="3">
-        <v>167.86000000000001</v>
+        <v>74.554500000000004</v>
       </c>
       <c r="C56" s="3">
-        <v>-88.530000000000001</v>
+        <v>-143.94319300000001</v>
       </c>
       <c r="D56" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E56" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="13.5">
       <c r="A57" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>D10</t>
         </is>
       </c>
       <c r="B57" s="3">
-        <v>64.236500000000007</v>
+        <v>70.796499999999995</v>
       </c>
       <c r="C57" s="3">
-        <v>-113.643693</v>
+        <v>-124.543693</v>
       </c>
       <c r="D57" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E57" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="13.5">
       <c r="A58" t="inlineStr">
         <is>
-          <t>J4</t>
+          <t>D11</t>
         </is>
       </c>
       <c r="B58" s="3">
-        <v>146.64993699999999</v>
+        <v>170.78999999999999</v>
       </c>
       <c r="C58" s="3">
-        <v>-68.622200000000007</v>
+        <v>-93.370000000000005</v>
       </c>
       <c r="D58" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E58" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="13.5">
       <c r="A59" t="inlineStr">
         <is>
-          <t>J6</t>
+          <t>D12</t>
         </is>
       </c>
       <c r="B59" s="3">
-        <v>173.47</v>
+        <v>157.28</v>
       </c>
       <c r="C59" s="3">
-        <v>-129.02000000000001</v>
+        <v>-93.392499999999998</v>
       </c>
       <c r="D59" s="3">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E59" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13.5">
       <c r="A60" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B60" s="3">
-        <v>92.754499999999993</v>
+        <v>64.236500000000007</v>
       </c>
       <c r="C60" s="3">
-        <v>-120.427693</v>
+        <v>-113.643693</v>
       </c>
       <c r="D60" s="3">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E60" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13.5">
       <c r="A61" t="inlineStr">
         <is>
-          <t>L2</t>
+          <t>J4</t>
         </is>
       </c>
       <c r="B61" s="3">
-        <v>95.802499999999995</v>
+        <v>146.64993699999999</v>
       </c>
       <c r="C61" s="3">
-        <v>-139.09669299999999</v>
+        <v>-68.622200000000007</v>
       </c>
       <c r="D61" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E61" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13.5">
       <c r="A62" t="inlineStr">
         <is>
-          <t>L3</t>
+          <t>J6</t>
         </is>
       </c>
       <c r="B62" s="3">
-        <v>163.58250000000001</v>
+        <v>173.47</v>
       </c>
       <c r="C62" s="3">
-        <v>-98.640000000000001</v>
+        <v>-129.02000000000001</v>
       </c>
       <c r="D62" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E62" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="13.5">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>J9</t>
         </is>
       </c>
       <c r="B63" s="3">
-        <v>67.046499999999995</v>
+        <v>151.159559</v>
       </c>
       <c r="C63" s="3">
-        <v>-125.793693</v>
+        <v>-61.5</v>
       </c>
       <c r="D63" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E63" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="13.5">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>J10</t>
         </is>
       </c>
       <c r="B64" s="3">
-        <v>159.17250000000001</v>
+        <v>190.08000000000001</v>
       </c>
       <c r="C64" s="3">
-        <v>-111.48999999999999</v>
+        <v>-52.159999999999997</v>
       </c>
       <c r="D64" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E64" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="13.5">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Q3</t>
+          <t>J11</t>
         </is>
       </c>
       <c r="B65" s="3">
-        <v>86.896500000000003</v>
+        <v>67.519999999999996</v>
       </c>
       <c r="C65" s="3">
-        <v>-105.568693</v>
+        <v>-88.694999999999993</v>
       </c>
       <c r="D65" s="3">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E65" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="13.5">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Q4</t>
+          <t>J12</t>
         </is>
       </c>
       <c r="B66" s="3">
-        <v>86.796499999999995</v>
+        <v>60.223999999999997</v>
       </c>
       <c r="C66" s="3">
-        <v>-112.543693</v>
+        <v>-67.349999999999994</v>
       </c>
       <c r="D66" s="3">
         <v>-90</v>
       </c>
       <c r="E66" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="13.5">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Q5</t>
+          <t>L1</t>
         </is>
       </c>
       <c r="B67" s="3">
-        <v>151.36250000000001</v>
+        <v>92.754499999999993</v>
       </c>
       <c r="C67" s="3">
-        <v>-111.48999999999999</v>
+        <v>-120.427693</v>
       </c>
       <c r="D67" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E67" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="13.5">
       <c r="A68" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>L2</t>
         </is>
       </c>
       <c r="B68" s="3">
-        <v>85.996499999999997</v>
+        <v>95.802499999999995</v>
       </c>
       <c r="C68" s="3">
-        <v>-109.068693</v>
+        <v>-139.09669299999999</v>
       </c>
       <c r="D68" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E68" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="13.5">
       <c r="A69" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>L3</t>
         </is>
       </c>
       <c r="B69" s="3">
-        <v>72.6965</v>
+        <v>175.49000000000001</v>
       </c>
       <c r="C69" s="3">
-        <v>-119.643693</v>
+        <v>-98.340000000000003</v>
       </c>
       <c r="D69" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13.5">
       <c r="A70" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>L4</t>
         </is>
       </c>
       <c r="B70" s="3">
-        <v>72.246499999999997</v>
+        <v>162</v>
       </c>
       <c r="C70" s="3">
-        <v>-140.343693</v>
+        <v>-98.340000000000003</v>
       </c>
       <c r="D70" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="13.5">
       <c r="A71" t="inlineStr">
         <is>
-          <t>R4</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="B71" s="3">
-        <v>108.9965</v>
+        <v>67.046499999999995</v>
       </c>
       <c r="C71" s="3">
-        <v>-111.943693</v>
+        <v>-125.793693</v>
       </c>
       <c r="D71" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="13.5">
       <c r="A72" t="inlineStr">
         <is>
-          <t>R5</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="B72" s="3">
-        <v>94.496499999999997</v>
+        <v>86.896500000000003</v>
       </c>
       <c r="C72" s="3">
-        <v>-106.74369299999999</v>
+        <v>-105.568693</v>
       </c>
       <c r="D72" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E72" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="13.5">
       <c r="A73" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>Q4</t>
         </is>
       </c>
       <c r="B73" s="3">
-        <v>108.9965</v>
+        <v>86.796499999999995</v>
       </c>
       <c r="C73" s="3">
-        <v>-110.143693</v>
+        <v>-112.543693</v>
       </c>
       <c r="D73" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E73" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="13.5">
       <c r="A74" t="inlineStr">
         <is>
-          <t>R7</t>
+          <t>R1</t>
         </is>
       </c>
       <c r="B74" s="3">
-        <v>72.6965</v>
+        <v>85.996499999999997</v>
       </c>
       <c r="C74" s="3">
-        <v>-108.343693</v>
+        <v>-109.068693</v>
       </c>
       <c r="D74" s="3">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E74" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="13.5">
       <c r="A75" t="inlineStr">
         <is>
-          <t>R8</t>
+          <t>R2</t>
         </is>
       </c>
       <c r="B75" s="3">
-        <v>74.554500000000004</v>
+        <v>72.6965</v>
       </c>
       <c r="C75" s="3">
-        <v>-140.343693</v>
+        <v>-119.643693</v>
       </c>
       <c r="D75" s="3">
         <v>-90</v>
       </c>
       <c r="E75" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="13.5">
       <c r="A76" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="B76" s="3">
-        <v>71.4465</v>
+        <v>72.246499999999997</v>
       </c>
       <c r="C76" s="3">
-        <v>-128.49369300000001</v>
+        <v>-140.343693</v>
       </c>
       <c r="D76" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E76" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="13.5">
       <c r="A77" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R4</t>
         </is>
       </c>
       <c r="B77" s="3">
-        <v>145.79650000000001</v>
+        <v>108.9965</v>
       </c>
       <c r="C77" s="3">
-        <v>-138.943693</v>
+        <v>-111.943693</v>
       </c>
       <c r="D77" s="3">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E77" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="13.5">
       <c r="A78" t="inlineStr">
         <is>
-          <t>R11</t>
+          <t>R5</t>
         </is>
       </c>
       <c r="B78" s="3">
-        <v>87.596500000000006</v>
+        <v>94.496499999999997</v>
       </c>
       <c r="C78" s="3">
-        <v>-109.068693</v>
+        <v>-106.74369299999999</v>
       </c>
       <c r="D78" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E78" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="13.5">
       <c r="A79" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="B79" s="3">
-        <v>146.90000000000001</v>
+        <v>108.9965</v>
       </c>
       <c r="C79" s="3">
-        <v>-75.650000000000006</v>
+        <v>-110.143693</v>
       </c>
       <c r="D79" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E79" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="13.5">
       <c r="A80" t="inlineStr">
         <is>
-          <t>R13</t>
+          <t>R7</t>
         </is>
       </c>
       <c r="B80" s="3">
-        <v>169.49250000000001</v>
+        <v>72.6965</v>
       </c>
       <c r="C80" s="3">
-        <v>-91.409999999999997</v>
+        <v>-108.343693</v>
       </c>
       <c r="D80" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E80" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="13.5">
       <c r="A81" t="inlineStr">
         <is>
-          <t>R14</t>
+          <t>R8</t>
         </is>
       </c>
       <c r="B81" s="3">
-        <v>94.496499999999997</v>
+        <v>74.554500000000004</v>
       </c>
       <c r="C81" s="3">
-        <v>-109.943693</v>
+        <v>-140.343693</v>
       </c>
       <c r="D81" s="3">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E81" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="13.5">
       <c r="A82" t="inlineStr">
         <is>
-          <t>R15</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="B82" s="3">
-        <v>108.9965</v>
+        <v>71.4465</v>
       </c>
       <c r="C82" s="3">
-        <v>-108.443693</v>
+        <v>-128.49369300000001</v>
       </c>
       <c r="D82" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E82" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="13.5">
       <c r="A83" t="inlineStr">
         <is>
-          <t>R16</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="B83" s="3">
-        <v>94.496499999999997</v>
+        <v>145.79650000000001</v>
       </c>
       <c r="C83" s="3">
-        <v>-108.343693</v>
+        <v>-138.943693</v>
       </c>
       <c r="D83" s="3">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E83" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5">
       <c r="A84" t="inlineStr">
         <is>
-          <t>R17</t>
+          <t>R11</t>
         </is>
       </c>
       <c r="B84" s="3">
-        <v>169.49250000000001</v>
+        <v>87.596500000000006</v>
       </c>
       <c r="C84" s="3">
-        <v>-95.890000000000001</v>
+        <v>-109.068693</v>
       </c>
       <c r="D84" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E84" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="13.5">
       <c r="A85" t="inlineStr">
         <is>
-          <t>R18</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="B85" s="3">
-        <v>107.1777</v>
+        <v>146.90000000000001</v>
       </c>
       <c r="C85" s="3">
-        <v>-139.190293</v>
+        <v>-75.650000000000006</v>
       </c>
       <c r="D85" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E85" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="13.5">
       <c r="A86" t="inlineStr">
         <is>
-          <t>R19</t>
+          <t>R13</t>
         </is>
       </c>
       <c r="B86" s="3">
-        <v>87.9285</v>
+        <v>178.52000000000001</v>
       </c>
       <c r="C86" s="3">
-        <v>-129.825693</v>
+        <v>-91.599999999999994</v>
       </c>
       <c r="D86" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E86" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="13.5">
       <c r="A87" t="inlineStr">
         <is>
-          <t>R20</t>
+          <t>R14</t>
         </is>
       </c>
       <c r="B87" s="3">
-        <v>84.626499999999993</v>
+        <v>94.496499999999997</v>
       </c>
       <c r="C87" s="3">
-        <v>-129.825693</v>
+        <v>-109.943693</v>
       </c>
       <c r="D87" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="13.5">
       <c r="A88" t="inlineStr">
         <is>
-          <t>R21</t>
+          <t>R15</t>
         </is>
       </c>
       <c r="B88" s="3">
-        <v>67.717500000000001</v>
+        <v>108.9965</v>
       </c>
       <c r="C88" s="3">
-        <v>-140.569693</v>
+        <v>-108.443693</v>
       </c>
       <c r="D88" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="13.5">
       <c r="A89" t="inlineStr">
         <is>
-          <t>R22</t>
+          <t>R16</t>
         </is>
       </c>
       <c r="B89" s="3">
-        <v>67.717500000000001</v>
+        <v>94.496499999999997</v>
       </c>
       <c r="C89" s="3">
-        <v>-143.843693</v>
+        <v>-108.343693</v>
       </c>
       <c r="D89" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="13.5">
       <c r="A90" t="inlineStr">
         <is>
-          <t>R23</t>
+          <t>R17</t>
         </is>
       </c>
       <c r="B90" s="3">
-        <v>87.9285</v>
+        <v>164.66999999999999</v>
       </c>
       <c r="C90" s="3">
-        <v>-132.111693</v>
+        <v>-91.599999999999994</v>
       </c>
       <c r="D90" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E90" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="13.5">
       <c r="A91" t="inlineStr">
         <is>
-          <t>R24</t>
+          <t>R18</t>
         </is>
       </c>
       <c r="B91" s="3">
-        <v>84.626499999999993</v>
+        <v>107.1777</v>
       </c>
       <c r="C91" s="3">
-        <v>-132.111693</v>
+        <v>-139.190293</v>
       </c>
       <c r="D91" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E91" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5">
       <c r="A92" t="inlineStr">
         <is>
-          <t>R25</t>
+          <t>R19</t>
         </is>
       </c>
       <c r="B92" s="3">
-        <v>159.66</v>
+        <v>87.9285</v>
       </c>
       <c r="C92" s="3">
-        <v>-115.20999999999999</v>
+        <v>-129.825693</v>
       </c>
       <c r="D92" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E92" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="13.5">
       <c r="A93" t="inlineStr">
         <is>
-          <t>R26</t>
+          <t>R20</t>
         </is>
       </c>
       <c r="B93" s="3">
-        <v>196.95500000000001</v>
+        <v>84.626499999999993</v>
       </c>
       <c r="C93" s="3">
-        <v>-129.27500000000001</v>
+        <v>-129.825693</v>
       </c>
       <c r="D93" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E93" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="13.5">
       <c r="A94" t="inlineStr">
         <is>
-          <t>R27</t>
+          <t>R21</t>
         </is>
       </c>
       <c r="B94" s="3">
-        <v>171.19</v>
+        <v>67.717500000000001</v>
       </c>
       <c r="C94" s="3">
-        <v>-122.59</v>
+        <v>-140.569693</v>
       </c>
       <c r="D94" s="3">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E94" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="13.5">
       <c r="A95" t="inlineStr">
         <is>
-          <t>R28</t>
+          <t>R22</t>
         </is>
       </c>
       <c r="B95" s="3">
-        <v>173.66499999999999</v>
+        <v>67.717500000000001</v>
       </c>
       <c r="C95" s="3">
-        <v>-118.69</v>
+        <v>-143.843693</v>
       </c>
       <c r="D95" s="3">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E95" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="13.5">
       <c r="A96" t="inlineStr">
         <is>
-          <t>R29</t>
+          <t>R23</t>
         </is>
       </c>
       <c r="B96" s="3">
-        <v>195.22999999999999</v>
+        <v>87.9285</v>
       </c>
       <c r="C96" s="3">
-        <v>-115.848</v>
+        <v>-132.111693</v>
       </c>
       <c r="D96" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E96" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="13.5">
       <c r="A97" t="inlineStr">
         <is>
-          <t>R30</t>
+          <t>R24</t>
         </is>
       </c>
       <c r="B97" s="3">
-        <v>187.45500000000001</v>
+        <v>84.626499999999993</v>
       </c>
       <c r="C97" s="3">
-        <v>-112.43000000000001</v>
+        <v>-132.111693</v>
       </c>
       <c r="D97" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E97" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="13.5">
       <c r="A98" t="inlineStr">
         <is>
-          <t>R31</t>
+          <t>R25</t>
         </is>
       </c>
       <c r="B98" s="3">
-        <v>65.346500000000006</v>
+        <v>80.920000000000002</v>
       </c>
       <c r="C98" s="3">
-        <v>-122.24369299999999</v>
+        <v>-90.719999999999999</v>
       </c>
       <c r="D98" s="3">
         <v>180</v>
       </c>
       <c r="E98" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="13.5">
       <c r="A99" t="inlineStr">
         <is>
-          <t>R32</t>
+          <t>R26</t>
         </is>
       </c>
       <c r="B99" s="3">
-        <v>116.59650000000001</v>
+        <v>196.95500000000001</v>
       </c>
       <c r="C99" s="3">
-        <v>-111.818693</v>
+        <v>-129.27500000000001</v>
       </c>
       <c r="D99" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E99" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="13.5">
       <c r="A100" t="inlineStr">
         <is>
-          <t>R33</t>
+          <t>R27</t>
         </is>
       </c>
       <c r="B100" s="3">
-        <v>108.9965</v>
+        <v>171.19</v>
       </c>
       <c r="C100" s="3">
-        <v>-106.693693</v>
+        <v>-122.59</v>
       </c>
       <c r="D100" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="13.5">
       <c r="A101" t="inlineStr">
         <is>
-          <t>R34</t>
+          <t>R28</t>
         </is>
       </c>
       <c r="B101" s="3">
-        <v>156.34</v>
+        <v>173.66499999999999</v>
       </c>
       <c r="C101" s="3">
-        <v>-115.20999999999999</v>
+        <v>-118.69</v>
       </c>
       <c r="D101" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="13.5">
       <c r="A102" t="inlineStr">
         <is>
-          <t>R35</t>
+          <t>R29</t>
         </is>
       </c>
       <c r="B102" s="3">
-        <v>149.06999999999999</v>
+        <v>195.22999999999999</v>
       </c>
       <c r="C102" s="3">
-        <v>-115.20999999999999</v>
+        <v>-115.848</v>
       </c>
       <c r="D102" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="13.5">
       <c r="A103" t="inlineStr">
         <is>
-          <t>R36</t>
+          <t>R30</t>
         </is>
       </c>
       <c r="B103" s="3">
-        <v>152.44499999999999</v>
+        <v>187.45500000000001</v>
       </c>
       <c r="C103" s="3">
-        <v>-115.20999999999999</v>
+        <v>-112.43000000000001</v>
       </c>
       <c r="D103" s="3">
         <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="13.5">
       <c r="A104" t="inlineStr">
         <is>
-          <t>TH1</t>
+          <t>R31</t>
         </is>
       </c>
       <c r="B104" s="3">
-        <v>109.2097</v>
+        <v>65.346500000000006</v>
       </c>
       <c r="C104" s="3">
-        <v>-139.190293</v>
+        <v>-122.24369299999999</v>
       </c>
       <c r="D104" s="3">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E104" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="13.5">
       <c r="A105" t="inlineStr">
         <is>
-          <t>U1</t>
+          <t>R32</t>
         </is>
       </c>
       <c r="B105" s="3">
-        <v>113.8965</v>
+        <v>116.59650000000001</v>
       </c>
       <c r="C105" s="3">
-        <v>-126.74369299999999</v>
+        <v>-111.818693</v>
       </c>
       <c r="D105" s="3">
         <v>-90</v>
       </c>
       <c r="E105" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="13.5">
       <c r="A106" t="inlineStr">
         <is>
-          <t>U2</t>
+          <t>R33</t>
         </is>
       </c>
       <c r="B106" s="3">
-        <v>101.7465</v>
+        <v>108.9965</v>
       </c>
       <c r="C106" s="3">
-        <v>-109.30619299999999</v>
+        <v>-106.693693</v>
       </c>
       <c r="D106" s="3">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E106" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="13.5">
       <c r="A107" t="inlineStr">
         <is>
-          <t>U3</t>
+          <t>R34</t>
         </is>
       </c>
       <c r="B107" s="3">
-        <v>100.12050000000001</v>
+        <v>80.909999999999997</v>
       </c>
       <c r="C107" s="3">
-        <v>-129.57169300000001</v>
+        <v>-83.030000000000001</v>
       </c>
       <c r="D107" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="13.5">
       <c r="A108" t="inlineStr">
         <is>
-          <t>U4</t>
+          <t>RN1</t>
         </is>
       </c>
       <c r="B108" s="3">
-        <v>73.496499999999997</v>
+        <v>80.831500000000005</v>
       </c>
       <c r="C108" s="3">
-        <v>-112.343693</v>
+        <v>-86.570188999999999</v>
       </c>
       <c r="D108" s="3">
         <v>0</v>
       </c>
       <c r="E108" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="13.5">
       <c r="A109" t="inlineStr">
         <is>
-          <t>U5</t>
+          <t>TH1</t>
         </is>
       </c>
       <c r="B109" s="3">
-        <v>77.296499999999995</v>
+        <v>109.2097</v>
       </c>
       <c r="C109" s="3">
-        <v>-122.143693</v>
+        <v>-139.190293</v>
       </c>
       <c r="D109" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E109" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="13.5">
       <c r="A110" t="inlineStr">
         <is>
-          <t>U6</t>
+          <t>U1</t>
         </is>
       </c>
       <c r="B110" s="3">
-        <v>164.4425</v>
+        <v>113.8965</v>
       </c>
       <c r="C110" s="3">
-        <v>-93.200000000000003</v>
+        <v>-126.74369299999999</v>
       </c>
       <c r="D110" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E110" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="13.5">
       <c r="A111" t="inlineStr">
         <is>
-          <t>U7</t>
+          <t>U2</t>
         </is>
       </c>
       <c r="B111" s="3">
-        <v>120.2465</v>
+        <v>101.7465</v>
       </c>
       <c r="C111" s="3">
-        <v>-111.943693</v>
+        <v>-109.30619299999999</v>
       </c>
       <c r="D111" s="3">
         <v>-90</v>
       </c>
       <c r="E111" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="13.5">
       <c r="A112" t="inlineStr">
         <is>
-          <t>U8</t>
+          <t>U3</t>
         </is>
       </c>
       <c r="B112" s="3">
-        <v>131.82149999999999</v>
+        <v>100.12050000000001</v>
       </c>
       <c r="C112" s="3">
-        <v>-131.79369299999999</v>
+        <v>-129.57169300000001</v>
       </c>
       <c r="D112" s="3">
         <v>180</v>
       </c>
       <c r="E112" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="13.5">
       <c r="A113" t="inlineStr">
         <is>
-          <t>U9</t>
+          <t>U4</t>
         </is>
       </c>
       <c r="B113" s="3">
-        <v>79.996499999999997</v>
+        <v>73.496499999999997</v>
       </c>
       <c r="C113" s="3">
-        <v>-110.543693</v>
+        <v>-112.343693</v>
       </c>
       <c r="D113" s="3">
         <v>0</v>
       </c>
       <c r="E113" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="13.5">
       <c r="A114" t="inlineStr">
         <is>
-          <t>U10</t>
+          <t>U5</t>
         </is>
       </c>
       <c r="B114" s="3">
-        <v>184.94999999999999</v>
+        <v>77.296499999999995</v>
       </c>
       <c r="C114" s="3">
-        <v>-120.70999999999999</v>
+        <v>-122.143693</v>
       </c>
       <c r="D114" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E114" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="13.5">
       <c r="A115" t="inlineStr">
         <is>
-          <t>U11</t>
+          <t>U6</t>
         </is>
       </c>
       <c r="B115" s="3">
-        <v>70.496499999999997</v>
+        <v>174.66</v>
       </c>
       <c r="C115" s="3">
-        <v>-133.48469299999999</v>
+        <v>-91.75</v>
       </c>
       <c r="D115" s="3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E115" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="13.5">
       <c r="A116" t="inlineStr">
         <is>
+          <t>U7</t>
+        </is>
+      </c>
+      <c r="B116" s="3">
+        <v>120.2465</v>
+      </c>
+      <c r="C116" s="3">
+        <v>-111.943693</v>
+      </c>
+      <c r="D116" s="3">
+        <v>-90</v>
+      </c>
+      <c r="E116" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="13.5">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>U8</t>
+        </is>
+      </c>
+      <c r="B117" s="3">
+        <v>131.82149999999999</v>
+      </c>
+      <c r="C117" s="3">
+        <v>-131.79369299999999</v>
+      </c>
+      <c r="D117" s="3">
+        <v>180</v>
+      </c>
+      <c r="E117" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="13.5">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>U9</t>
+        </is>
+      </c>
+      <c r="B118" s="3">
+        <v>79.996499999999997</v>
+      </c>
+      <c r="C118" s="3">
+        <v>-110.543693</v>
+      </c>
+      <c r="D118" s="3">
+        <v>0</v>
+      </c>
+      <c r="E118" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="13.5">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>U10</t>
+        </is>
+      </c>
+      <c r="B119" s="3">
+        <v>184.94999999999999</v>
+      </c>
+      <c r="C119" s="3">
+        <v>-120.70999999999999</v>
+      </c>
+      <c r="D119" s="3">
+        <v>0</v>
+      </c>
+      <c r="E119" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="13.5">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>U11</t>
+        </is>
+      </c>
+      <c r="B120" s="3">
+        <v>70.496499999999997</v>
+      </c>
+      <c r="C120" s="3">
+        <v>-133.48469299999999</v>
+      </c>
+      <c r="D120" s="3">
+        <v>-90</v>
+      </c>
+      <c r="E120" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="13.5">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>U12</t>
+        </is>
+      </c>
+      <c r="B121" s="3">
+        <v>161.16999999999999</v>
+      </c>
+      <c r="C121" s="3">
+        <v>-91.75</v>
+      </c>
+      <c r="D121" s="3">
+        <v>90</v>
+      </c>
+      <c r="E121" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="13.5">
+      <c r="A122" t="inlineStr">
+        <is>
           <t>Y1</t>
         </is>
       </c>
-      <c r="B116" s="3">
+      <c r="B122" s="3">
         <v>120.1465</v>
       </c>
-      <c r="C116" s="3">
+      <c r="C122" s="3">
         <v>-105.893693</v>
       </c>
-      <c r="D116" s="3">
-        <v>0</v>
-      </c>
-      <c r="E116" t="s">
-        <v>0</v>
+      <c r="D122" s="3">
+        <v>0</v>
+      </c>
+      <c r="E122" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>